<commit_message>
Large Language Model tools for R
</commit_message>
<xml_diff>
--- a/tables/modeling.xlsx
+++ b/tables/modeling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@Quarto projects/Rsources_book/Resources/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@GitProjects/@2024/rsources-book/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF96E00F-08DE-244E-AF76-08FB521A23ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41426DD9-9C5C-AE4F-BE01-91703E8B4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="14180" xr2:uid="{A71D1E1F-2EF4-304F-B366-595227DED5AF}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>author</t>
   </si>
@@ -368,6 +368,15 @@
   </si>
   <si>
     <t>Efficient Machine Learning with R (in progress)</t>
+  </si>
+  <si>
+    <t>Luis D. Verde Arregoitia</t>
+  </si>
+  <si>
+    <t>Large Language Model tools for R</t>
+  </si>
+  <si>
+    <t>https://luisdva.github.io/llmsr-book/</t>
   </si>
 </sst>
 </file>
@@ -723,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FEED76-E7A5-3C4A-A3C7-90B796B0A8E8}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,114 +778,114 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -884,284 +893,295 @@
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>